<commit_message>
added ymodem [builed failed]
</commit_message>
<xml_diff>
--- a/bootloader.xlsx
+++ b/bootloader.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\Keil\stm32_ota_bootloader\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8F8F633-CE61-40C4-B403-DB61BD99DF87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4165EC35-E796-4F31-AA9F-B6C40B239465}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="address" sheetId="1" r:id="rId1"/>
+    <sheet name="flow" sheetId="2" r:id="rId2"/>
+    <sheet name="QA" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
   <si>
     <t>Flash</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -63,10 +65,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>0x80010000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>0x10000</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -75,10 +73,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>pagge 1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>pagge 64</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -93,13 +87,139 @@
   <si>
     <t>FLASH</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bootloader</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>APP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>misc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x0800FC00 ~ 0x08010000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x08010000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pagge 20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>… …</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x08005000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x08000000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x08004FFF</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0800FFBFF</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fl</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>读取MISC分区的信息</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>？  0xCAFEBABE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>check</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CMD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0xBEEFBEEF</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>uart传输bin固件</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>问题</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. Flash 的读写操作</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2. uart 固件传输</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>check_misc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>get_args</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>finish_update</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>install_firmware</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>解锁FLASH</t>
+  </si>
+  <si>
+    <t>擦除FLASH</t>
+  </si>
+  <si>
+    <t>写入数据到FLASH</t>
+  </si>
+  <si>
+    <t>锁住FLASH</t>
+  </si>
+  <si>
+    <r>
+      <t>要写的页里有数据，要先读出来在缓存区，再把页擦除，再写入数据；在擦除页之后，只要这次你写的数据大小不够一页，可以连续写入</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>。</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -130,8 +250,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -150,6 +282,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="11">
     <border>
@@ -277,12 +427,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -308,6 +455,24 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -444,6 +609,735 @@
         <a:p>
           <a:pPr algn="l"/>
           <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>203638</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>145926</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>282466</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>28597</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="图片 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99C127D0-501B-4E4D-8258-A0F3767DFB6F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="203638" y="1334909"/>
+          <a:ext cx="3685190" cy="2825567"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>28574</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>666750</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="椭圆 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BB8D46B4-1BE8-4A94-BC6E-A42CE1332843}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3457574" y="2971800"/>
+          <a:ext cx="1323976" cy="447675"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>start</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>676275</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="矩形: 圆角 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53C4C221-C594-458F-AE0B-46F0EBF1B183}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3419475" y="3886200"/>
+          <a:ext cx="1381125" cy="428625"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:t>初始化</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>676275</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>66676</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="菱形 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0E56B754-AD3D-4480-AD91-7B9FCCA91339}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="4876800"/>
+          <a:ext cx="1362075" cy="619126"/>
+        </a:xfrm>
+        <a:prstGeom prst="diamond">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>MISC</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>681038</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>4762</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="直接箭头连接符 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{05E8E36A-F09F-4195-886A-5A9528DE13E9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="2" idx="4"/>
+          <a:endCxn id="3" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="4110038" y="3419475"/>
+          <a:ext cx="9524" cy="466725"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>681038</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>681038</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="直接箭头连接符 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{383F8A4C-9151-4E71-B77B-977611DFE3AF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="3" idx="2"/>
+          <a:endCxn id="4" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4110038" y="4314825"/>
+          <a:ext cx="0" cy="561975"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>676275</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="矩形: 圆角 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8BCB0DA8-CB1B-490C-A80A-73EC99E74D99}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3419475" y="6343650"/>
+          <a:ext cx="1381125" cy="428625"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:t>启动</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>APP</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>681038</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>66676</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>681038</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="直接箭头连接符 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{957970AC-33F6-474B-812F-B3FF06EC23D2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="4" idx="2"/>
+          <a:endCxn id="10" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4110038" y="5495926"/>
+          <a:ext cx="0" cy="847724"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="20" name="矩形: 圆角 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B5F7977A-C48D-4F16-B7F0-99781D34D78D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5743575" y="4991100"/>
+          <a:ext cx="1381125" cy="428625"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:t>升级</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>676275</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>119063</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>138113</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="23" name="直接箭头连接符 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{274085BD-8826-46CF-9AF8-D0B5EA9CE876}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="4" idx="3"/>
+          <a:endCxn id="20" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4791075" y="5186363"/>
+          <a:ext cx="952500" cy="19050"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>66674</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="29" name="连接符: 肘形 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE775B77-595C-4BA7-B671-03B3B10129A8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000" flipV="1">
+          <a:off x="4143375" y="5495924"/>
+          <a:ext cx="2266950" cy="371476"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 420"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>666750</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>676275</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="32" name="矩形: 圆角 31">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{330FC16C-8AE6-4A10-AF64-F229527D7E68}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3409950" y="7248525"/>
+          <a:ext cx="1381125" cy="428625"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:t>修改异常向量表</a:t>
+          </a:r>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -715,10 +1609,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A4:H35"/>
+  <dimension ref="A4:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -730,10 +1624,13 @@
     <col min="6" max="6" width="5" customWidth="1"/>
     <col min="7" max="7" width="8.75" customWidth="1"/>
     <col min="8" max="8" width="8.625" customWidth="1"/>
+    <col min="9" max="9" width="10.125" customWidth="1"/>
+    <col min="10" max="10" width="22.875" customWidth="1"/>
+    <col min="12" max="12" width="13.375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="21" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -744,7 +1641,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="3"/>
+      <c r="A5" s="21"/>
       <c r="B5" s="2" t="s">
         <v>2</v>
       </c>
@@ -753,167 +1650,213 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="E9" s="20" t="s">
+      <c r="E9" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="G9" s="4"/>
-      <c r="H9" s="5"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="4"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E10" s="1"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="7"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="6"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E11" s="1"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="7"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="6"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E12" s="1"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="7"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="6"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G13" s="16"/>
-      <c r="H13" s="17"/>
+        <v>12</v>
+      </c>
+      <c r="G13" s="15"/>
+      <c r="H13" s="16"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E14" s="1"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="15"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="14"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="E15" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="G15" s="14" t="s">
+      <c r="E15" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="H15" s="15"/>
+      <c r="H15" s="14"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E16" s="1"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="15"/>
-    </row>
-    <row r="17" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="G16" s="13"/>
+      <c r="H16" s="14"/>
+    </row>
+    <row r="17" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E17" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G17" s="18"/>
-      <c r="H17" s="19"/>
-    </row>
-    <row r="18" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="G17" s="17"/>
+      <c r="H17" s="18"/>
+    </row>
+    <row r="18" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E18" s="1"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="7"/>
-    </row>
-    <row r="19" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="G18" s="5"/>
+      <c r="H18" s="6"/>
+    </row>
+    <row r="19" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E19" s="1"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="7"/>
-    </row>
-    <row r="20" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="G19" s="5"/>
+      <c r="H19" s="6"/>
+    </row>
+    <row r="20" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E20" s="1"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="7"/>
-    </row>
-    <row r="21" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="G20" s="5"/>
+      <c r="H20" s="6"/>
+    </row>
+    <row r="21" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E21" s="1"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="7"/>
-    </row>
-    <row r="22" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="G21" s="5"/>
+      <c r="H21" s="6"/>
+    </row>
+    <row r="22" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E22" s="1"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="7"/>
-    </row>
-    <row r="23" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="G22" s="5"/>
+      <c r="H22" s="6"/>
+    </row>
+    <row r="23" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E23" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G23" s="9"/>
+      <c r="H23" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="I23" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="J23" t="s">
+        <v>18</v>
+      </c>
+      <c r="K23" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E24" s="1"/>
+      <c r="G24" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H24" s="10"/>
+      <c r="I24" s="24"/>
+      <c r="J24" t="s">
+        <v>25</v>
+      </c>
+      <c r="K24" s="27"/>
+    </row>
+    <row r="25" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E25" s="1"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="24"/>
+      <c r="K25" s="27"/>
+    </row>
+    <row r="26" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E26" s="1"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="K26" s="27">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="27" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E27" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="G23" s="10"/>
-      <c r="H23" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="24" spans="5:8" x14ac:dyDescent="0.2">
-      <c r="E24" s="1"/>
-      <c r="G24" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="H24" s="11"/>
-    </row>
-    <row r="25" spans="5:8" x14ac:dyDescent="0.2">
-      <c r="E25" s="1"/>
-      <c r="G25" s="12"/>
-      <c r="H25" s="11"/>
-    </row>
-    <row r="26" spans="5:8" x14ac:dyDescent="0.2">
-      <c r="E26" s="1"/>
-      <c r="G26" s="12"/>
-      <c r="H26" s="11"/>
-    </row>
-    <row r="27" spans="5:8" x14ac:dyDescent="0.2">
-      <c r="E27" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="G27" s="12" t="s">
+      <c r="G27" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="H27" s="11"/>
-    </row>
-    <row r="28" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="H27" s="10"/>
+      <c r="I27" s="24"/>
+      <c r="K27" s="27"/>
+    </row>
+    <row r="28" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E28" s="1"/>
-      <c r="G28" s="12"/>
-      <c r="H28" s="11"/>
-    </row>
-    <row r="29" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="G28" s="11"/>
+      <c r="H28" s="10"/>
+      <c r="I28" s="24"/>
+      <c r="J28" t="s">
+        <v>22</v>
+      </c>
+      <c r="K28" s="27"/>
+    </row>
+    <row r="29" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E29" s="1"/>
-      <c r="G29" s="12"/>
-      <c r="H29" s="11"/>
-    </row>
-    <row r="30" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="G29" s="11"/>
+      <c r="H29" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="I29" s="23"/>
+      <c r="J29" t="s">
+        <v>24</v>
+      </c>
+      <c r="K29" s="27"/>
+    </row>
+    <row r="30" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E30" s="1"/>
-      <c r="G30" s="12"/>
-      <c r="H30" s="11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="31" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="G30" s="11"/>
+      <c r="H30" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="I30" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="K30" s="27">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E31" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G31" s="13"/>
-      <c r="H31" s="11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="32" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="G31" s="12"/>
+      <c r="H31" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="I31" s="23"/>
+      <c r="J31" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E32" s="1"/>
-      <c r="G32" s="6"/>
-      <c r="H32" s="7"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="6"/>
     </row>
     <row r="33" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E33" s="1"/>
-      <c r="G33" s="6"/>
-      <c r="H33" s="7"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="6"/>
     </row>
     <row r="34" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E34" s="1"/>
-      <c r="G34" s="6"/>
-      <c r="H34" s="7"/>
+      <c r="G34" s="5"/>
+      <c r="H34" s="6"/>
     </row>
     <row r="35" spans="5:8" x14ac:dyDescent="0.2">
-      <c r="E35" s="20" t="s">
+      <c r="E35" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="G35" s="8"/>
-      <c r="H35" s="9"/>
+      <c r="G35" s="7"/>
+      <c r="H35" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -924,4 +1867,130 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967294" verticalDpi="4294967294" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98CEC4D3-D430-40C6-9E43-6D0DBB6922C9}">
+  <dimension ref="A1:P32"/>
+  <sheetViews>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="P20" sqref="P20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="16" max="16" width="16.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="3:16" x14ac:dyDescent="0.2">
+      <c r="N19" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="3:16" x14ac:dyDescent="0.2">
+      <c r="O20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="3:16" x14ac:dyDescent="0.2">
+      <c r="O21" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="3:16" x14ac:dyDescent="0.2">
+      <c r="O26" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="3:16" x14ac:dyDescent="0.2">
+      <c r="O27" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="3:16" x14ac:dyDescent="0.2">
+      <c r="L28" t="s">
+        <v>32</v>
+      </c>
+      <c r="P28" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" spans="3:16" x14ac:dyDescent="0.2">
+      <c r="D29" t="s">
+        <v>27</v>
+      </c>
+      <c r="P29" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31" spans="3:16" x14ac:dyDescent="0.2">
+      <c r="C31" t="s">
+        <v>29</v>
+      </c>
+      <c r="D31" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="3:16" x14ac:dyDescent="0.2">
+      <c r="C32" t="s">
+        <v>30</v>
+      </c>
+      <c r="D32" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C16C59E9-B6E0-4617-8B18-3ED7E5447BBE}">
+  <dimension ref="B4:D9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="28" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="D5" s="28" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="D6" s="28" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="D7" s="28" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C9" s="28" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>